<commit_message>
A lot of progress through reaper and fmod
</commit_message>
<xml_diff>
--- a/Documentation/Asset List.xlsx
+++ b/Documentation/Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolStuff\RIT 3 Spring\AudioFinalProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9AFA61-6F63-4A58-9406-15FECB135F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69484F09-8E98-4B9F-904F-1835C4FA6A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14355" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{FCB6DF7E-CC76-4F1F-AF37-7D1819E0D10B}"/>
+    <workbookView xWindow="0" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{FCB6DF7E-CC76-4F1F-AF37-7D1819E0D10B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Sound</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Synthy sound that descends</t>
+  </si>
+  <si>
+    <t>FMOD</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
   <dimension ref="B3:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +727,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>57</v>
@@ -844,7 +847,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>38</v>
@@ -864,7 +867,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>46</v>
@@ -966,7 +969,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>39</v>
@@ -986,7 +989,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1006,7 +1009,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
@@ -1026,7 +1029,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>42</v>
@@ -1086,7 +1089,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>50</v>
@@ -1106,7 +1109,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>44</v>
@@ -1212,7 +1215,7 @@
         <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Unity update, audio production, and resources
</commit_message>
<xml_diff>
--- a/Documentation/Asset List.xlsx
+++ b/Documentation/Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolStuff\RIT 3 Spring\AudioFinalProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69484F09-8E98-4B9F-904F-1835C4FA6A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34939D0C-896B-4D56-8F97-389C381DEA48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{FCB6DF7E-CC76-4F1F-AF37-7D1819E0D10B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Sound</t>
   </si>
@@ -250,6 +250,18 @@
   </si>
   <si>
     <t>FMOD</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Unity Integration</t>
+  </si>
+  <si>
+    <t>Coin pickup</t>
+  </si>
+  <si>
+    <t>bone-like crunch</t>
   </si>
 </sst>
 </file>
@@ -271,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +305,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -345,6 +387,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21BAF2-86B3-4FF6-816A-A7F546253339}">
   <dimension ref="B3:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +751,7 @@
       <c r="B4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -726,8 +773,8 @@
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
+      <c r="C5" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>57</v>
@@ -748,7 +795,7 @@
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -786,7 +833,7 @@
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -806,7 +853,7 @@
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -826,7 +873,7 @@
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="1"/>
@@ -846,8 +893,8 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>72</v>
+      <c r="C11" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>38</v>
@@ -866,8 +913,8 @@
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>72</v>
+      <c r="C12" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>46</v>
@@ -886,7 +933,7 @@
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -906,7 +953,7 @@
       <c r="B14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -928,7 +975,7 @@
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="1"/>
@@ -948,7 +995,7 @@
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="1"/>
@@ -968,8 +1015,8 @@
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
+      <c r="C17" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>39</v>
@@ -988,8 +1035,8 @@
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>72</v>
+      <c r="C18" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1008,8 +1055,8 @@
       <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>72</v>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
@@ -1028,8 +1075,8 @@
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>72</v>
+      <c r="C20" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>42</v>
@@ -1068,7 +1115,7 @@
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1088,8 +1135,8 @@
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>72</v>
+      <c r="C23" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>50</v>
@@ -1108,8 +1155,8 @@
       <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>72</v>
+      <c r="C24" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>44</v>
@@ -1128,7 +1175,7 @@
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="1"/>
@@ -1148,7 +1195,7 @@
       <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1182,7 +1229,7 @@
       <c r="B28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1198,7 +1245,7 @@
       <c r="B29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1214,8 +1261,8 @@
       <c r="B30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>72</v>
+      <c r="C30" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>54</v>
@@ -1230,8 +1277,8 @@
       <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>45</v>
+      <c r="C31" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>71</v>
@@ -1243,10 +1290,18 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Lots of updates that have not been pushed
</commit_message>
<xml_diff>
--- a/Documentation/Asset List.xlsx
+++ b/Documentation/Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolStuff\RIT 3 Spring\AudioFinalProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D6556-13CF-417F-BFCF-97AAFF3F6E46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274944DE-BD47-4931-8B25-91A193337D19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCB6DF7E-CC76-4F1F-AF37-7D1819E0D10B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
   <si>
     <t>Sound</t>
   </si>
@@ -219,24 +219,12 @@
     <t>hard time finding fitting sounds. Maybe record?</t>
   </si>
   <si>
-    <t>later priority. Other sounds are more important to implement right now</t>
-  </si>
-  <si>
-    <t>later priority. Not doing music until sound work is almost done</t>
-  </si>
-  <si>
-    <t>later priority. Hard time thinking of noise I would like for this one. The game did not have a noise for it either.</t>
-  </si>
-  <si>
     <t>Powerup Pickup</t>
   </si>
   <si>
     <t>finding assets</t>
   </si>
   <si>
-    <t>switched from "magnet pickup" to be all items</t>
-  </si>
-  <si>
     <t>Powerup End</t>
   </si>
   <si>
@@ -258,9 +246,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -303,13 +288,19 @@
     <t>ExtraLife</t>
   </si>
   <si>
-    <t>Unity</t>
-  </si>
-  <si>
     <t>chimes</t>
   </si>
   <si>
     <t>could not make a good sound so using regular button press</t>
+  </si>
+  <si>
+    <t>pulled from existing project</t>
+  </si>
+  <si>
+    <t>Game Music</t>
+  </si>
+  <si>
+    <t>taken out. Hard to find a spot in code to que sound</t>
   </si>
 </sst>
 </file>
@@ -331,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,25 +355,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -436,9 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,14 +426,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -777,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21BAF2-86B3-4FF6-816A-A7F546253339}">
-  <dimension ref="B3:L46"/>
+  <dimension ref="B3:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +773,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
@@ -826,11 +796,11 @@
       <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>74</v>
+      <c r="C4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>57</v>
@@ -840,7 +810,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -851,11 +821,11 @@
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>74</v>
+      <c r="C5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>56</v>
@@ -864,7 +834,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>59</v>
@@ -878,11 +848,11 @@
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>74</v>
+      <c r="C6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>33</v>
@@ -902,7 +872,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
         <v>18</v>
@@ -920,11 +890,11 @@
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>74</v>
+      <c r="C8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>60</v>
@@ -943,11 +913,11 @@
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>75</v>
+      <c r="C9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>37</v>
@@ -967,16 +937,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -987,11 +957,11 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>74</v>
+      <c r="C11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>38</v>
@@ -1000,7 +970,7 @@
         <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="2"/>
@@ -1012,11 +982,11 @@
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>74</v>
+      <c r="C12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>46</v>
@@ -1025,7 +995,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="2"/>
@@ -1040,7 +1010,7 @@
       <c r="C13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1055,24 +1025,22 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>67</v>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1084,17 +1052,19 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1105,17 +1075,19 @@
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1123,23 +1095,21 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>74</v>
+        <v>88</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1148,22 +1118,22 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>74</v>
+        <v>7</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
@@ -1173,22 +1143,22 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>74</v>
+        <v>36</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
@@ -1198,44 +1168,50 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H20" s="1"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
-        <v>43</v>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1243,23 +1219,19 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1267,23 +1239,21 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>74</v>
+        <v>11</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>86</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1292,22 +1262,22 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>74</v>
+        <v>13</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="2"/>
@@ -1317,96 +1287,100 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="G25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="B26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4" t="s">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>74</v>
+        <v>31</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>18</v>
@@ -1416,95 +1390,107 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="4" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H32" s="1"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="11"/>
+      <c r="D35" s="8"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1513,7 +1499,7 @@
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="D36" s="8"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1609,14 +1595,23 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D4:D35">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="yes">
+  <conditionalFormatting sqref="D4:D36">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>